<commit_message>
Added my GitHub repository link to the Excel sheet
</commit_message>
<xml_diff>
--- a/Git_repo_info.xlsx
+++ b/Git_repo_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Training\IIHT\Wipro_July_2025\wiprojulytrain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOHAM TANAVADE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D4D45A-548B-442C-9406-AFAA8DF2A304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DB8D63-8413-4B65-B32A-957B7ACD3D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D5FD5A7F-D155-4FC6-8FC7-23616F485FD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5FD5A7F-D155-4FC6-8FC7-23616F485FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Git Repo" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="162">
   <si>
     <t>S No</t>
   </si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>https://github.com/Ashok-web784/wiproconfig</t>
+  </si>
+  <si>
+    <t>https://github.com/soham0608/WiproTraining_Assignments</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1258,8 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1776,6 +1779,9 @@
       <c r="B56" s="12" t="s">
         <v>65</v>
       </c>
+      <c r="C56" s="19" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
@@ -1941,9 +1947,10 @@
     <hyperlink ref="C38" r:id="rId3" tooltip="https://github.com/deekshithamunigala/java_full_stack" xr:uid="{8DBE9A31-F653-4A6B-9B68-25403E3F0D9F}"/>
     <hyperlink ref="C52" r:id="rId4" xr:uid="{76AEAEAC-0FA7-4ABC-97D4-A71438FA545E}"/>
     <hyperlink ref="C29" r:id="rId5" tooltip="https://github.com/ashok-web784/wiproconfig" xr:uid="{8BB3790F-EED2-46B3-B368-01F32BD64347}"/>
+    <hyperlink ref="C56" r:id="rId6" xr:uid="{0710DEAF-C701-42D8-992E-5C84EE3C50AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>